<commit_message>
Clean up regression code
</commit_message>
<xml_diff>
--- a/etc/mvw-test-data.xlsx
+++ b/etc/mvw-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\METools\method-eval-tools\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0336CB4F-E12C-4E00-94FC-B6216D0CFDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DDC948-57D1-491D-BE74-8983CB9B635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="420" windowWidth="22275" windowHeight="19110" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13875" yWindow="795" windowWidth="22275" windowHeight="19110" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comp 1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="235">
   <si>
     <t>Reference Method</t>
   </si>
@@ -940,6 +940,9 @@
   </si>
   <si>
     <t>EP05_A1</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -6302,8 +6305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D70B62E-C183-4D29-A9A9-387646CEF91A}">
   <dimension ref="A1:Y167"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8218,8 +8221,14 @@
       <c r="O32" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -8251,7 +8260,7 @@
         <v>3.7627484960896122E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -8302,8 +8311,15 @@
         <f>POWER(M34*J34,2)/G34</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <v>20</v>
+      </c>
+      <c r="Q34">
+        <f>(P34-1)/($G$28-3)</f>
+        <v>0.24675324675324675</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -8354,8 +8370,15 @@
         <f t="shared" ref="O35:O36" si="18">POWER(M35*J35,2)/G35</f>
         <v>2.051693698158585E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <v>2</v>
+      </c>
+      <c r="Q35">
+        <f>(P35-1)/($G$28-3)</f>
+        <v>1.2987012987012988E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -8406,8 +8429,15 @@
         <f t="shared" si="18"/>
         <v>1.4916638367065273E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <v>2</v>
+      </c>
+      <c r="Q36">
+        <f>(P36-1)/($G$28-3)</f>
+        <v>1.2987012987012988E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -8421,7 +8451,7 @@
         <v>102.18390876234</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -8442,7 +8472,7 @@
         <v>0.19966203281116524</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -8463,7 +8493,7 @@
         <v>3.5433575348651123E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -8484,7 +8514,7 @@
         <v>56.34826032839667</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -8498,7 +8528,7 @@
         <v>95.755952301741203</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -8512,7 +8542,7 @@
         <v>106.64351196067599</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -8526,7 +8556,7 @@
         <v>98.852209551491597</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -8540,7 +8570,7 @@
         <v>99.493433384858406</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -8554,7 +8584,7 @@
         <v>98.634645392121001</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -8568,7 +8598,7 @@
         <v>99.262354950237295</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -8582,7 +8612,7 @@
         <v>99.053648233066596</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -10769,7 +10799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C36204-48D9-454C-9744-8C8F9C4F181A}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>